<commit_message>
Adding Enumeration, EnumerationLiterals refsets.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,24 +4,26 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
-    <sheet name="Foundation Metadata" sheetId="10" r:id="rId2"/>
+    <sheet name="Foundation Metadata" sheetId="11" r:id="rId2"/>
     <sheet name="FHIMModelsRS" sheetId="9" r:id="rId3"/>
     <sheet name="FHIMClassesRS" sheetId="2" r:id="rId4"/>
-    <sheet name="FHIMAttributesRS" sheetId="5" r:id="rId5"/>
-    <sheet name="FHIMDefaultValuesRS" sheetId="8" r:id="rId6"/>
-    <sheet name="FHIMRelationshipsRS" sheetId="4" r:id="rId7"/>
-    <sheet name="FHIMConstraintsRS" sheetId="7" r:id="rId8"/>
+    <sheet name="FHIMEnumerationRS" sheetId="10" r:id="rId5"/>
+    <sheet name="FHIMEnumerationValuesRS" sheetId="12" r:id="rId6"/>
+    <sheet name="FHIMAttributesRS" sheetId="5" r:id="rId7"/>
+    <sheet name="FHIMDefaultValuesRS" sheetId="8" r:id="rId8"/>
+    <sheet name="FHIMRelationshipsRS" sheetId="4" r:id="rId9"/>
+    <sheet name="FHIMConstraintsRS" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="114">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -164,60 +166,6 @@
     <t>Dependency</t>
   </si>
   <si>
-    <t>BloodPressureBodySite :: Left Arm</t>
-  </si>
-  <si>
-    <t>BloodPressureBodySite :: Left Leg</t>
-  </si>
-  <si>
-    <t>BloodPressureBodySite :: Right Arm</t>
-  </si>
-  <si>
-    <t>BloodPressureBodySite :: Right leg</t>
-  </si>
-  <si>
-    <t>BloodPressureCuffSize :: AdultCuff</t>
-  </si>
-  <si>
-    <t>BloodPressureCuffSize :: LargeAdultCuff</t>
-  </si>
-  <si>
-    <t>BloodPressureCuffSize :: PediatricCuff</t>
-  </si>
-  <si>
-    <t>BloodPressureCuffSize :: SmallAdultCuff</t>
-  </si>
-  <si>
-    <t>BloodPressureCuffSize :: ThighCuff</t>
-  </si>
-  <si>
-    <t>BloodPressureMethod :: CuffAutomated</t>
-  </si>
-  <si>
-    <t>BloodPressureMethod :: CuffManual</t>
-  </si>
-  <si>
-    <t>BloodPressureMethod :: Doppler</t>
-  </si>
-  <si>
-    <t>BloodPressureMethod :: NonInvasive</t>
-  </si>
-  <si>
-    <t>BloodPressureMethod :: Palpated</t>
-  </si>
-  <si>
-    <t>BloodPressurePosition :: Lying</t>
-  </si>
-  <si>
-    <t>BloodPressurePosition :: SemiFowlers</t>
-  </si>
-  <si>
-    <t>BloodPressurePosition :: Sitting</t>
-  </si>
-  <si>
-    <t>BloodPressurePosition :: Standing</t>
-  </si>
-  <si>
     <t>BloodPressure</t>
   </si>
   <si>
@@ -339,6 +287,84 @@
   </si>
   <si>
     <t>attributeType (CID)</t>
+  </si>
+  <si>
+    <t>memberID for BloodPressureBodySite Enumeration</t>
+  </si>
+  <si>
+    <t>memberID for BloodPressureCuffSize Enumeration</t>
+  </si>
+  <si>
+    <t>memberID for BloodPressureMethod Enumeration</t>
+  </si>
+  <si>
+    <t>memberID for BloodPressurePosition Enumeration</t>
+  </si>
+  <si>
+    <t>componentID for BloodPressureBodySite Enumeration</t>
+  </si>
+  <si>
+    <t>componentID for BloodPressureCuffSize Enumeration</t>
+  </si>
+  <si>
+    <t>componentID for BloodPressureMethod Enumeration</t>
+  </si>
+  <si>
+    <t>componentID for BloodPressurePosition Enumeration</t>
+  </si>
+  <si>
+    <t>LeftArm</t>
+  </si>
+  <si>
+    <t>RightArm</t>
+  </si>
+  <si>
+    <t>LeftLeg</t>
+  </si>
+  <si>
+    <t>RightLeg</t>
+  </si>
+  <si>
+    <t>AdultCuff</t>
+  </si>
+  <si>
+    <t>LargeAdultCuff</t>
+  </si>
+  <si>
+    <t>PediatricCuff</t>
+  </si>
+  <si>
+    <t>SmallAdultCuff</t>
+  </si>
+  <si>
+    <t>ThighCuff</t>
+  </si>
+  <si>
+    <t>CuffAutomated</t>
+  </si>
+  <si>
+    <t>CuffManual</t>
+  </si>
+  <si>
+    <t>Doppler</t>
+  </si>
+  <si>
+    <t>NonInvasive</t>
+  </si>
+  <si>
+    <t>Palpated</t>
+  </si>
+  <si>
+    <t>Lying</t>
+  </si>
+  <si>
+    <t>SemiFowlers</t>
+  </si>
+  <si>
+    <t>Standing</t>
+  </si>
+  <si>
+    <t>Sitting</t>
   </si>
 </sst>
 </file>
@@ -822,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -885,7 +911,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,7 +923,7 @@
       </c>
       <c r="C8" s="7"/>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -914,7 +940,7 @@
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -927,12 +953,12 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>0</v>
@@ -943,10 +969,10 @@
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -966,7 +992,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -977,7 +1003,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1001,7 +1027,7 @@
         <v>35</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1026,7 +1052,7 @@
         <v>36</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1034,7 +1060,7 @@
     </row>
     <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="C28" s="6"/>
     </row>
@@ -1052,10 +1078,10 @@
         <v>5</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1065,157 +1091,176 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.88671875" customWidth="1"/>
+    <col min="1" max="1" width="78.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.88671875" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A9">
-    <sortCondition ref="A2:A9"/>
+  <sortState ref="A1:A9">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1249,13 +1294,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1305,7 +1350,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,7 +1377,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -1340,24 +1385,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1365,7 +1410,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
@@ -1376,7 +1421,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1387,7 +1432,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
@@ -1395,13 +1440,13 @@
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1411,10 +1456,281 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:1" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <sortState ref="A2:A9">
+    <sortCondition ref="A2:A9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="46.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1437,7 +1753,7 @@
         <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>31</v>
@@ -1445,7 +1761,7 @@
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>42</v>
@@ -1462,7 +1778,7 @@
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>42</v>
@@ -1479,10 +1795,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
@@ -1496,10 +1812,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -1513,10 +1829,10 @@
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -1530,13 +1846,13 @@
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>42</v>
@@ -1544,21 +1860,21 @@
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>43</v>
@@ -1567,15 +1883,13 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>43</v>
@@ -1584,15 +1898,13 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
         <v>44</v>
@@ -1609,7 +1921,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>44</v>
@@ -1618,15 +1930,13 @@
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>37</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>45</v>
@@ -1643,7 +1953,7 @@
     </row>
     <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>45</v>
@@ -1652,18 +1962,15 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>34</v>
@@ -1677,16 +1984,16 @@
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>37</v>
@@ -1738,7 +2045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1771,18 +2078,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1790,12 +2097,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1833,7 +2140,7 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
@@ -1844,7 +2151,7 @@
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>23</v>
@@ -1869,7 +2176,7 @@
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -1917,29 +2224,29 @@
         <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>37</v>
@@ -1953,10 +2260,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1967,10 +2271,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1981,10 +2282,7 @@
         <v>46</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1995,10 +2293,7 @@
         <v>46</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -2007,112 +2302,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="78.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="45.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updating Foundation Metadata tab to reflect implementation.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Blood pressure taking (procedure)</t>
   </si>
   <si>
-    <t>Generalization</t>
-  </si>
-  <si>
     <t>AbstractBloodPressureObservation</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Multiplicity</t>
   </si>
   <si>
-    <t>Association</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
   </si>
   <si>
     <t>componentID for BloodPressurePositionQualifier Class</t>
-  </si>
-  <si>
-    <t>Dependency</t>
   </si>
   <si>
     <t>BloodPressure</t>
@@ -909,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>13</v>
@@ -951,7 +942,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -963,7 +954,7 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -980,7 +971,7 @@
     </row>
     <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -993,12 +984,12 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>0</v>
@@ -1009,10 +1000,10 @@
     </row>
     <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
@@ -1020,7 +1011,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2"/>
     </row>
@@ -1032,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,7 +1034,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1053,7 +1044,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1064,10 +1055,10 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1078,7 +1069,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
@@ -1089,10 +1080,10 @@
         <v>5</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1100,13 +1091,13 @@
     </row>
     <row r="28" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>3</v>
@@ -1118,10 +1109,10 @@
         <v>5</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1151,78 +1142,78 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1237,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1254,71 +1245,71 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1351,38 +1342,38 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1392,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,47 +1397,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1485,13 +1466,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1565,10 +1546,10 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1576,43 +1557,43 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1620,10 +1601,10 @@
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
@@ -1631,13 +1612,13 @@
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1673,10 +1654,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
@@ -1684,21 +1665,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -1706,13 +1687,13 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1764,151 +1745,151 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1944,18 +1925,18 @@
         <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1964,15 +1945,15 @@
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1981,15 +1962,15 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -1998,15 +1979,15 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -2015,15 +1996,15 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
@@ -2032,177 +2013,177 @@
         <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -2264,12 +2245,12 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2277,18 +2258,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2316,18 +2297,18 @@
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
@@ -2335,10 +2316,10 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
@@ -2346,10 +2327,10 @@
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C4" s="9">
         <v>1</v>
@@ -2357,10 +2338,10 @@
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -2368,10 +2349,10 @@
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C6" s="11">
         <v>0</v>
@@ -2379,10 +2360,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" s="11">
         <v>1</v>
@@ -2390,10 +2371,10 @@
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C8" s="11">
         <v>0</v>
@@ -2401,10 +2382,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C9" s="11">
         <v>1</v>
@@ -2412,10 +2393,10 @@
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C10" s="11">
         <v>0</v>
@@ -2423,10 +2404,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C11" s="11">
         <v>1</v>
@@ -2434,10 +2415,10 @@
     </row>
     <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C12" s="11">
         <v>0</v>
@@ -2445,10 +2426,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C13" s="11">
         <v>1</v>
@@ -2456,10 +2437,10 @@
     </row>
     <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C14" s="11">
         <v>0</v>
@@ -2467,10 +2448,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" s="11">
         <v>1</v>

</xml_diff>

<commit_message>
Correcting an error on 'Dependencies' tab.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,7 +1303,7 @@
         <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>57</v>
@@ -1385,7 +1385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changing Dependency refset to be of type CidCidStr.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="121">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -1226,89 +1226,108 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="49.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="49.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
+    <col min="3" max="4" width="49.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parsing refset members into Associations in ISAAC model.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="FHIMGeneralizationsRS" sheetId="4" r:id="rId10"/>
     <sheet name="FHIMDependenciesRS" sheetId="14" r:id="rId11"/>
     <sheet name="FHIMAssociationsRS" sheetId="13" r:id="rId12"/>
+    <sheet name="FHIMAssociationEndsRS" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="124">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -366,28 +368,37 @@
     <t>target (CID)</t>
   </si>
   <si>
-    <t>ownedEnd (CID)</t>
-  </si>
-  <si>
     <t>client (CID)</t>
   </si>
   <si>
     <t>supplier (CID)</t>
   </si>
   <si>
-    <t>unownedEnd (CID)</t>
-  </si>
-  <si>
     <t>memberID for dbpo_bpo Association</t>
   </si>
   <si>
-    <t>memberID for unnamed bloodPressureObservation Attribute</t>
-  </si>
-  <si>
     <t>componentID for unnamed bloodPressureObservation Attribute</t>
   </si>
   <si>
     <t>memberID for sbpo_bpo Association</t>
+  </si>
+  <si>
+    <t>memberEnd (CID)</t>
+  </si>
+  <si>
+    <t>owned (Boolean)</t>
+  </si>
+  <si>
+    <t>componentID for dbpo_bpo Association</t>
+  </si>
+  <si>
+    <t>componentID for sbpo_bpo Association</t>
+  </si>
+  <si>
+    <t>memberID for dbpo_bpo Association ownedEnd</t>
+  </si>
+  <si>
+    <t>memberID for sbpo_bpo Association ownedEnd</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1249,10 +1260,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>25</v>
@@ -1338,22 +1349,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" style="2" customWidth="1"/>
     <col min="2" max="2" width="49.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="76.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="13.109375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -1361,38 +1371,105 @@
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>76</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1539,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1920,8 +1997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2193,7 +2270,7 @@
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>42</v>
@@ -2206,9 +2283,19 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="E19" s="2"/>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>

</xml_diff>

<commit_message>
Addiing FHIM visibility, making sure exported file can be imported.
</commit_message>
<xml_diff>
--- a/resources/fhim/FHIM_dbp_refSetMapping.xlsx
+++ b/resources/fhim/FHIM_dbp_refSetMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="758" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="source" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,18 @@
     <sheet name="FHIMAttributesRS" sheetId="5" r:id="rId7"/>
     <sheet name="FHIMDefaultValuesRS" sheetId="8" r:id="rId8"/>
     <sheet name="FHIMMultiplicityRS" sheetId="7" r:id="rId9"/>
-    <sheet name="FHIMGeneralizationsRS" sheetId="4" r:id="rId10"/>
-    <sheet name="FHIMDependenciesRS" sheetId="14" r:id="rId11"/>
-    <sheet name="FHIMAssociationsRS" sheetId="13" r:id="rId12"/>
-    <sheet name="FHIMAssociationEndsRS" sheetId="15" r:id="rId13"/>
+    <sheet name="FHIMVisibilityRS" sheetId="16" r:id="rId10"/>
+    <sheet name="FHIMGeneralizationsRS" sheetId="4" r:id="rId11"/>
+    <sheet name="FHIMDependenciesRS" sheetId="14" r:id="rId12"/>
+    <sheet name="FHIMAssociationsRS" sheetId="13" r:id="rId13"/>
+    <sheet name="FHIMAssociationEndsRS" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="129">
   <si>
     <t>DiastolicBloodPressureObservation</t>
   </si>
@@ -399,6 +399,21 @@
   </si>
   <si>
     <t>memberID for sbpo_bpo Association ownedEnd</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>componentID for dbpo_bpo Association ownedEnd</t>
+  </si>
+  <si>
+    <t>componentID for sbpo_bpo Association ownedEnd</t>
+  </si>
+  <si>
+    <t>visibilityType (String)</t>
   </si>
 </sst>
 </file>
@@ -1135,6 +1150,162 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="78.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1235,7 +1406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1347,7 +1518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1401,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1997,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2388,7 +2559,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A17" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>